<commit_message>
Dodanie Prezentacji ale trzeba poprawić
</commit_message>
<xml_diff>
--- a/etap2/Zadanie Dodatkowe/Oferty_Internet_Polska.xlsx
+++ b/etap2/Zadanie Dodatkowe/Oferty_Internet_Polska.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9B903D-A070-49F1-8FBD-C0A8E0547BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="21">
   <si>
     <t>Operator</t>
   </si>
@@ -64,92 +70,29 @@
     <t>500 Mb/s</t>
   </si>
   <si>
-    <t>69,99 zł</t>
-  </si>
-  <si>
-    <t>79,99 zł</t>
-  </si>
-  <si>
-    <t>89,99 zł</t>
-  </si>
-  <si>
-    <t>99,00 zł netto</t>
-  </si>
-  <si>
-    <t>109,00 zł netto</t>
-  </si>
-  <si>
-    <t>125,00 zł netto</t>
-  </si>
-  <si>
-    <t>49,99 zł</t>
-  </si>
-  <si>
-    <t>59,99 zł</t>
-  </si>
-  <si>
-    <t>60,00 zł netto</t>
-  </si>
-  <si>
-    <t>70,00 zł netto</t>
-  </si>
-  <si>
-    <t>90,00 zł netto</t>
-  </si>
-  <si>
-    <t>65,00 zł</t>
-  </si>
-  <si>
-    <t>75,00 zł</t>
-  </si>
-  <si>
-    <t>85,00 zł</t>
-  </si>
-  <si>
-    <t>65,00 zł netto</t>
-  </si>
-  <si>
-    <t>75,00 zł netto</t>
-  </si>
-  <si>
-    <t>85,00 zł netto</t>
-  </si>
-  <si>
-    <t>74,90 zł</t>
-  </si>
-  <si>
-    <t>84,90 zł</t>
-  </si>
-  <si>
-    <t>94,90 zł</t>
-  </si>
-  <si>
-    <t>100,00 zł netto</t>
-  </si>
-  <si>
-    <t>110,00 zł netto</t>
-  </si>
-  <si>
-    <t>120,00 zł netto</t>
-  </si>
-  <si>
-    <t>95,00 zł netto</t>
-  </si>
-  <si>
-    <t>60,00 zł</t>
-  </si>
-  <si>
-    <t>70,00 zł</t>
-  </si>
-  <si>
-    <t>90,00 zł</t>
+    <t>Nasza Firma</t>
+  </si>
+  <si>
+    <t>900 Mb/s</t>
+  </si>
+  <si>
+    <t>KategoriaFirma</t>
+  </si>
+  <si>
+    <t>Inne</t>
+  </si>
+  <si>
+    <t>Nasza</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;zł&quot;;[Red]\-#,##0.00\ &quot;zł&quot;"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -197,28 +140,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -256,7 +223,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -290,6 +257,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -324,9 +292,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -499,14 +468,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,8 +495,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -530,11 +509,14 @@
       <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2" s="4">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -544,11 +526,14 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" s="4">
+        <v>79.989999999999995</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -558,25 +543,17 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D4" s="4">
+        <v>89.99</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -586,11 +563,14 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6" s="4">
+        <v>109</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -600,11 +580,14 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" s="4">
+        <v>125</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -614,11 +597,14 @@
       <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="4">
+        <v>49.99</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -628,11 +614,14 @@
       <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" s="4">
+        <v>59.99</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -642,25 +631,17 @@
       <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D10" s="4">
+        <v>89.99</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -670,11 +651,14 @@
       <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="D12" s="4">
+        <v>70</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -684,11 +668,14 @@
       <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="D13" s="4">
+        <v>90</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -698,11 +685,14 @@
       <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14" s="4">
+        <v>65</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -712,11 +702,14 @@
       <c r="C15" t="s">
         <v>13</v>
       </c>
-      <c r="D15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="D15" s="4">
+        <v>75</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -726,25 +719,17 @@
       <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="D16" s="4">
+        <v>85</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -754,11 +739,14 @@
       <c r="C18" t="s">
         <v>13</v>
       </c>
-      <c r="D18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="D18" s="4">
+        <v>75</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -768,11 +756,14 @@
       <c r="C19" t="s">
         <v>14</v>
       </c>
-      <c r="D19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="D19" s="4">
+        <v>85</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -782,11 +773,14 @@
       <c r="C20" t="s">
         <v>12</v>
       </c>
-      <c r="D20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="D20" s="4">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -796,11 +790,14 @@
       <c r="C21" t="s">
         <v>13</v>
       </c>
-      <c r="D21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="D21" s="4">
+        <v>84.9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -810,25 +807,17 @@
       <c r="C22" t="s">
         <v>14</v>
       </c>
-      <c r="D22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="D22" s="4">
+        <v>94.9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -838,11 +827,14 @@
       <c r="C24" t="s">
         <v>13</v>
       </c>
-      <c r="D24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="D24" s="4">
+        <v>110</v>
+      </c>
+      <c r="E24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -852,11 +844,14 @@
       <c r="C25" t="s">
         <v>14</v>
       </c>
-      <c r="D25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="D25" s="4">
+        <v>120</v>
+      </c>
+      <c r="E25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -866,11 +861,14 @@
       <c r="C26" t="s">
         <v>12</v>
       </c>
-      <c r="D26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="D26" s="4">
+        <v>59.99</v>
+      </c>
+      <c r="E26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -880,11 +878,14 @@
       <c r="C27" t="s">
         <v>13</v>
       </c>
-      <c r="D27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="D27" s="4">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="E27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -894,25 +895,17 @@
       <c r="C28" t="s">
         <v>14</v>
       </c>
-      <c r="D28" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="D28" s="4">
+        <v>89.99</v>
+      </c>
+      <c r="E28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -922,11 +915,14 @@
       <c r="C30" t="s">
         <v>13</v>
       </c>
-      <c r="D30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="D30" s="4">
+        <v>75</v>
+      </c>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -936,11 +932,14 @@
       <c r="C31" t="s">
         <v>14</v>
       </c>
-      <c r="D31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="D31" s="4">
+        <v>95</v>
+      </c>
+      <c r="E31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -950,11 +949,14 @@
       <c r="C32" t="s">
         <v>12</v>
       </c>
-      <c r="D32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="D32" s="4">
+        <v>60</v>
+      </c>
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -964,11 +966,14 @@
       <c r="C33" t="s">
         <v>13</v>
       </c>
-      <c r="D33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="D33" s="4">
+        <v>70</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -978,25 +983,17 @@
       <c r="C34" t="s">
         <v>14</v>
       </c>
-      <c r="D34" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="D34" s="4">
+        <v>90</v>
+      </c>
+      <c r="E34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1006,11 +1003,14 @@
       <c r="C36" t="s">
         <v>13</v>
       </c>
-      <c r="D36" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="D36" s="4">
+        <v>70</v>
+      </c>
+      <c r="E36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1020,8 +1020,96 @@
       <c r="C37" t="s">
         <v>14</v>
       </c>
-      <c r="D37" t="s">
-        <v>26</v>
+      <c r="D37" s="4">
+        <v>90</v>
+      </c>
+      <c r="E37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="4">
+        <v>60</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="4">
+        <v>70</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="4">
+        <v>80</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="4">
+        <v>105</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="4">
+        <v>119.99</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>